<commit_message>
Atualização das categorias e do arquivo de fluxo de caixa
</commit_message>
<xml_diff>
--- a/fluxo_de_caixa.xlsx
+++ b/fluxo_de_caixa.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,7 +454,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-09-01 19:36:22</t>
+          <t>2023-09-02 11:18:06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -464,140 +464,40 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vamos testar</t>
+          <t>Vamos ver</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Teste</t>
+          <t>Novo</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-09-01 19:36:49</t>
+          <t>2023-09-02 11:49:24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Saída</t>
+          <t>Entrada</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Quero ver</t>
+          <t>Vamos ver</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>-11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nao Tem</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-09-01 19:37:06</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Saída</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Oxi a pois</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>-66</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Nao Tem</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2023-09-01 20:07:22</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Entrada</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ewqewq</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>as</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2023-09-01 20:11:57</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Saída</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Varios</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>-10</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Nova</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2023-09-01 20:12:14</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Entrada</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>dsadsa</t>
+          <t>vamnos</t>
         </is>
       </c>
     </row>

</xml_diff>